<commit_message>
Added More to Collection
</commit_message>
<xml_diff>
--- a/CabinetFiles/Main-Tracker.xlsx
+++ b/CabinetFiles/Main-Tracker.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c91312bf17d42d6f/Desktop/liquor-cabinet/CabinetFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83DDCB51-7CB5-42E3-AF64-E97FD5941485}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14A61157-59B3-4FA1-9032-52C17625B501}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="2330" windowWidth="16470" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22180" windowHeight="14140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$D$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="79">
   <si>
     <t>Distillery</t>
   </si>
@@ -111,12 +114,6 @@
     <t>Rye</t>
   </si>
   <si>
-    <t>Sub Category 1</t>
-  </si>
-  <si>
-    <t>Subcategory 2</t>
-  </si>
-  <si>
     <t>Japanese</t>
   </si>
   <si>
@@ -172,6 +169,102 @@
   </si>
   <si>
     <t>Retired</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>SubCategory1</t>
+  </si>
+  <si>
+    <t>Subcategory2</t>
+  </si>
+  <si>
+    <t>Scotch</t>
+  </si>
+  <si>
+    <t>Islay</t>
+  </si>
+  <si>
+    <t>Ardbeg</t>
+  </si>
+  <si>
+    <t>An Oa</t>
+  </si>
+  <si>
+    <t>Uigeadail</t>
+  </si>
+  <si>
+    <t>Spectacular</t>
+  </si>
+  <si>
+    <t>Port Cask</t>
+  </si>
+  <si>
+    <t>American Single Malt</t>
+  </si>
+  <si>
+    <t>Virginia Distillery Co.</t>
+  </si>
+  <si>
+    <t>The Brewer's Coalition Goose Island Bourbon County Brand Stout Cask Finished</t>
+  </si>
+  <si>
+    <t>Lost Lantern</t>
+  </si>
+  <si>
+    <t>Flame</t>
+  </si>
+  <si>
+    <t>Blend of Sante Fe Spirits and Whiskey Del Bac</t>
+  </si>
+  <si>
+    <t>Westland</t>
+  </si>
+  <si>
+    <t>Sherry Wood</t>
+  </si>
+  <si>
+    <t>Washington, USA</t>
+  </si>
+  <si>
+    <t>Bourbon</t>
+  </si>
+  <si>
+    <t>Wildwood Spirits Co</t>
+  </si>
+  <si>
+    <t>The Dark Door</t>
+  </si>
+  <si>
+    <t>Heigold</t>
+  </si>
+  <si>
+    <t>Rest of World</t>
+  </si>
+  <si>
+    <t>Kavalan</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
+  </si>
+  <si>
+    <t>Classic Single Malt</t>
+  </si>
+  <si>
+    <t>Concertmaster - Port Cask</t>
+  </si>
+  <si>
+    <t>Concertmaster - Sherry Cask</t>
+  </si>
+  <si>
+    <t>King Car Conductor</t>
+  </si>
+  <si>
+    <t>Oloroso Sherry Oak</t>
+  </si>
+  <si>
+    <t>Port Oak</t>
   </si>
 </sst>
 </file>
@@ -210,10 +303,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,29 +588,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.26953125" customWidth="1"/>
+    <col min="2" max="2" width="26.26953125" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.90625" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -527,11 +625,11 @@
       <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J1" t="s">
         <v>4</v>
@@ -540,240 +638,609 @@
         <v>5</v>
       </c>
       <c r="L1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>26</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>31</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="K4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="I5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.46600000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
         <v>27</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="E11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.54200000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.46</v>
+      </c>
+      <c r="J12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1">
-        <v>0.43</v>
-      </c>
-      <c r="I2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="I5" t="s">
-        <v>47</v>
-      </c>
-      <c r="J5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0.43</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H14" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="1">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" t="s">
         <v>41</v>
       </c>
-      <c r="F8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="2">
-        <v>0.44500000000000001</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="K8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9">
-        <v>10</v>
-      </c>
-      <c r="E9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="1">
+      <c r="H17" s="2">
+        <v>0.47499999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" t="s">
+        <v>72</v>
+      </c>
+      <c r="H18" s="2">
         <v>0.4</v>
       </c>
-      <c r="I9" s="1"/>
+      <c r="L18" s="3">
+        <v>45839</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" t="s">
+        <v>72</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="L20" s="3">
+        <v>45839</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21" t="s">
+        <v>72</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" t="s">
+        <v>72</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" t="s">
+        <v>72</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0.54</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="B1:D1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D23">
+      <sortCondition ref="C1"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L23">
+    <sortCondition ref="B1:B23"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>